<commit_message>
new and improved spread sheet
</commit_message>
<xml_diff>
--- a/P05/docs/MASS_Scrum.xlsx
+++ b/P05/docs/MASS_Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/SCHOOL/UTA/CSE 1325/assignments/cse1325/P05/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2D8CE7-6346-7941-AD6C-13D3BBFBAED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921E403E-46B6-2045-BFDD-B2AAF8688CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="152">
   <si>
     <t>Product Name:</t>
   </si>
@@ -174,33 +174,6 @@
   </si>
   <si>
     <t>CAT</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Create and list cats (or 2</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>nd</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> animal family) as well</t>
-    </r>
   </si>
   <si>
     <r>
@@ -637,6 +610,31 @@
   <si>
     <t>Finished in Sprint 1</t>
   </si>
+  <si>
+    <r>
+      <t>Create and list cats (or 2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> animal family) as well</t>
+    </r>
+  </si>
+  <si>
+    <t>Create and list cats (or 2nd animal family) as well</t>
+  </si>
 </sst>
 </file>
 
@@ -647,7 +645,7 @@
     <numFmt numFmtId="165" formatCode="mmm\ dd"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -722,6 +720,12 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -804,7 +808,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -924,6 +928,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1443,28 +1451,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1679,7 +1687,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -1827,7 +1835,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -1901,7 +1909,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -1992,7 +2000,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2140,7 +2148,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2214,7 +2222,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -2305,7 +2313,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2453,7 +2461,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2527,7 +2535,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3460,8 +3468,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -3503,7 +3511,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="43"/>
       <c r="D2" s="43"/>
@@ -3549,7 +3557,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="44"/>
       <c r="D5" s="44"/>
@@ -3557,7 +3565,7 @@
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
       <c r="H5" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I5" s="5">
         <v>1001964490</v>
@@ -3896,7 +3904,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>31</v>
@@ -3929,7 +3937,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H25" s="17" t="s">
         <v>36</v>
@@ -3962,7 +3970,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H26" s="17" t="s">
         <v>36</v>
@@ -3995,24 +4003,24 @@
         <v>1</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>36</v>
       </c>
       <c r="I27" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="J27" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="18" t="s">
+      <c r="K27" s="18" t="s">
         <v>46</v>
-      </c>
-      <c r="K27" s="18" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="14">
       <c r="A28" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B28" s="21">
         <v>5</v>
@@ -4030,18 +4038,18 @@
         <v>31</v>
       </c>
       <c r="I28" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="J28" s="23" t="s">
+      <c r="K28" s="23" t="s">
         <v>50</v>
-      </c>
-      <c r="K28" s="23" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="14">
       <c r="A29" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="21">
         <v>6</v>
@@ -4059,18 +4067,18 @@
         <v>31</v>
       </c>
       <c r="I29" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J29" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="K29" s="23" t="s">
         <v>54</v>
-      </c>
-      <c r="K29" s="23" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="14">
       <c r="A30" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="21">
         <v>7</v>
@@ -4088,18 +4096,18 @@
         <v>31</v>
       </c>
       <c r="I30" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="J30" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="K30" s="23" t="s">
         <v>58</v>
-      </c>
-      <c r="K30" s="23" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="14">
       <c r="A31" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="21">
         <v>8</v>
@@ -4117,18 +4125,18 @@
         <v>31</v>
       </c>
       <c r="I31" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="J31" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="J31" s="23" t="s">
-        <v>62</v>
-      </c>
       <c r="K31" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="16">
       <c r="A32" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" s="21">
         <v>9</v>
@@ -4146,18 +4154,18 @@
         <v>36</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J32" s="23" t="s">
         <v>38</v>
       </c>
       <c r="K32" s="23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:1024" ht="16">
       <c r="A33" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" s="21">
         <v>10</v>
@@ -4175,18 +4183,18 @@
         <v>36</v>
       </c>
       <c r="I33" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="J33" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="J33" s="23" t="s">
+      <c r="K33" s="23" t="s">
         <v>68</v>
-      </c>
-      <c r="K33" s="23" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:1024" ht="42">
       <c r="A34" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" s="21">
         <v>11</v>
@@ -4204,18 +4212,18 @@
         <v>36</v>
       </c>
       <c r="I34" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="J34" s="23" t="s">
+      <c r="K34" s="23" t="s">
         <v>72</v>
-      </c>
-      <c r="K34" s="23" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:1024" s="24" customFormat="1" ht="28">
       <c r="A35" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B35" s="15">
         <v>12</v>
@@ -4230,21 +4238,21 @@
       <c r="F35" s="16"/>
       <c r="G35" s="16"/>
       <c r="H35" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="I35" s="18" t="s">
+      <c r="J35" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="J35" s="18" t="s">
+      <c r="K35" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="K35" s="18" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:1024" s="24" customFormat="1" ht="28">
       <c r="A36" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="15">
         <v>13</v>
@@ -4259,21 +4267,21 @@
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
       <c r="H36" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I36" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="J36" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="K36" s="18" t="s">
         <v>80</v>
-      </c>
-      <c r="J36" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="K36" s="18" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:1024" s="24" customFormat="1" ht="14">
       <c r="A37" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B37" s="15">
         <v>14</v>
@@ -4288,21 +4296,21 @@
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
       <c r="H37" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I37" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="I37" s="18" t="s">
+      <c r="J37" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="J37" s="18" t="s">
+      <c r="K37" s="18" t="s">
         <v>85</v>
-      </c>
-      <c r="K37" s="18" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:1024" s="24" customFormat="1" ht="14">
       <c r="A38" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B38" s="15">
         <v>15</v>
@@ -4317,21 +4325,21 @@
       <c r="F38" s="16"/>
       <c r="G38" s="16"/>
       <c r="H38" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I38" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="J38" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="J38" s="18" t="s">
+      <c r="K38" s="18" t="s">
         <v>89</v>
-      </c>
-      <c r="K38" s="18" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:1024" s="24" customFormat="1" ht="14">
       <c r="A39" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" s="15">
         <v>16</v>
@@ -4346,21 +4354,21 @@
       <c r="F39" s="16"/>
       <c r="G39" s="16"/>
       <c r="H39" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I39" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J39" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="J39" s="18" t="s">
+      <c r="K39" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="K39" s="18" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:1024" ht="28">
       <c r="A40" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B40" s="21">
         <v>17</v>
@@ -4378,13 +4386,13 @@
         <v>36</v>
       </c>
       <c r="I40" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="J40" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="K40" s="23" t="s">
         <v>97</v>
-      </c>
-      <c r="K40" s="23" t="s">
-        <v>98</v>
       </c>
       <c r="L40"/>
       <c r="M40"/>
@@ -5402,7 +5410,7 @@
     </row>
     <row r="41" spans="1:1024" ht="28">
       <c r="A41" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B41" s="21">
         <v>18</v>
@@ -5418,13 +5426,13 @@
       <c r="G41" s="16"/>
       <c r="H41" s="22"/>
       <c r="I41" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J41" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="J41" s="23" t="s">
+      <c r="K41" s="23" t="s">
         <v>101</v>
-      </c>
-      <c r="K41" s="23" t="s">
-        <v>102</v>
       </c>
       <c r="L41"/>
       <c r="M41"/>
@@ -6442,7 +6450,7 @@
     </row>
     <row r="42" spans="1:1024" ht="28">
       <c r="A42" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="21">
         <v>19</v>
@@ -6460,18 +6468,18 @@
         <v>36</v>
       </c>
       <c r="I42" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="J42" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="J42" s="23" t="s">
+      <c r="K42" s="23" t="s">
         <v>105</v>
-      </c>
-      <c r="K42" s="23" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:1024" ht="14">
       <c r="A43" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B43" s="21">
         <v>20</v>
@@ -6486,21 +6494,21 @@
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
       <c r="H43" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I43" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="I43" s="25" t="s">
+      <c r="J43" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="J43" s="25" t="s">
+      <c r="K43" s="23" t="s">
         <v>110</v>
-      </c>
-      <c r="K43" s="23" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:1024" s="24" customFormat="1" ht="14">
       <c r="A44" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B44" s="15">
         <v>21</v>
@@ -6515,21 +6523,21 @@
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
       <c r="H44" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I44" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="J44" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="J44" s="18" t="s">
+      <c r="K44" s="18" t="s">
         <v>114</v>
-      </c>
-      <c r="K44" s="18" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="45" spans="1:1024" s="24" customFormat="1" ht="28">
       <c r="A45" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B45" s="15">
         <v>22</v>
@@ -6547,13 +6555,13 @@
         <v>36</v>
       </c>
       <c r="I45" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="J45" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="J45" s="18" t="s">
+      <c r="K45" s="18" t="s">
         <v>118</v>
-      </c>
-      <c r="K45" s="18" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:1024" s="24" customFormat="1" ht="4.5" customHeight="1">
@@ -6579,21 +6587,21 @@
       <c r="G47" s="18"/>
       <c r="H47" s="18"/>
       <c r="I47" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J47" s="18"/>
       <c r="K47" s="18"/>
     </row>
     <row r="48" spans="1:1024" ht="28">
       <c r="A48" s="20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="21">
         <v>4</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E48" s="21">
         <v>5</v>
@@ -6601,28 +6609,28 @@
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
       <c r="H48" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I48" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="J48" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="J48" s="23" t="s">
+      <c r="K48" s="23" t="s">
         <v>124</v>
-      </c>
-      <c r="K48" s="23" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="24" customFormat="1" ht="28">
       <c r="A49" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="21">
         <v>4</v>
       </c>
       <c r="D49" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E49" s="21">
         <v>8</v>
@@ -6630,16 +6638,16 @@
       <c r="F49" s="16"/>
       <c r="G49" s="16"/>
       <c r="H49" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I49" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="J49" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="J49" s="23" t="s">
+      <c r="K49" s="23" t="s">
         <v>128</v>
-      </c>
-      <c r="K49" s="23" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -7350,8 +7358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="165" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -7381,14 +7389,14 @@
     </row>
     <row r="2" spans="1:1024" s="33" customFormat="1">
       <c r="A2" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="34">
         <v>44614</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -7397,7 +7405,7 @@
     </row>
     <row r="3" spans="1:1024" s="33" customFormat="1">
       <c r="A3" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="34">
         <f>B2+7</f>
@@ -7412,10 +7420,10 @@
     </row>
     <row r="4" spans="1:1024" s="33" customFormat="1">
       <c r="A4" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -7440,7 +7448,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
@@ -7450,11 +7458,10 @@
     </row>
     <row r="7" spans="1:1024" s="33" customFormat="1">
       <c r="A7" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="31">
-        <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
@@ -7465,14 +7472,13 @@
     </row>
     <row r="8" spans="1:1024" s="33" customFormat="1">
       <c r="A8" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="31">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C8" s="31">
-        <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
         <v>0</v>
       </c>
       <c r="D8" s="31"/>
@@ -7483,15 +7489,14 @@
     </row>
     <row r="9" spans="1:1024" s="33" customFormat="1">
       <c r="A9" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="31">
-        <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
@@ -7501,14 +7506,13 @@
     </row>
     <row r="10" spans="1:1024" s="33" customFormat="1">
       <c r="A10" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="31">
-        <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
         <v>0</v>
       </c>
       <c r="D10" s="31"/>
@@ -7519,14 +7523,13 @@
     </row>
     <row r="11" spans="1:1024" s="33" customFormat="1">
       <c r="A11" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="31">
-        <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
         <v>0</v>
       </c>
       <c r="D11" s="31"/>
@@ -7537,14 +7540,13 @@
     </row>
     <row r="12" spans="1:1024" s="33" customFormat="1">
       <c r="A12" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="31">
-        <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
         <v>0</v>
       </c>
       <c r="D12" s="31"/>
@@ -7555,14 +7557,13 @@
     </row>
     <row r="13" spans="1:1024" s="33" customFormat="1">
       <c r="A13" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="31">
-        <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
         <v>0</v>
       </c>
       <c r="D13" s="31"/>
@@ -7573,14 +7574,13 @@
     </row>
     <row r="14" spans="1:1024" s="33" customFormat="1">
       <c r="A14" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="31">
-        <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
         <v>0</v>
       </c>
       <c r="D14" s="31"/>
@@ -7601,16 +7601,16 @@
     </row>
     <row r="16" spans="1:1024">
       <c r="A16" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="38" t="s">
         <v>144</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>145</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>25</v>
@@ -7623,9 +7623,14 @@
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" s="39"/>
-      <c r="D17" s="40" t="s">
-        <v>146</v>
+      <c r="B17" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>32</v>
       </c>
       <c r="E17" s="41"/>
     </row>
@@ -7633,24 +7638,45 @@
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" s="39"/>
-      <c r="D18" s="39"/>
+      <c r="B18" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="39" t="s">
+        <v>37</v>
+      </c>
       <c r="E18" s="41"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19">
         <v>3</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="D19" s="39"/>
+      <c r="B19" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="39" t="s">
+        <v>41</v>
+      </c>
       <c r="E19" s="41"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="D20" s="39"/>
+      <c r="B20" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="39" t="s">
+        <v>151</v>
+      </c>
       <c r="E20" s="41"/>
     </row>
     <row r="21" spans="1:5">
@@ -8294,13 +8320,9 @@
       <c r="E100" s="41"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="4">
     <dataValidation operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Task ID" prompt="This is just an arbitrary unique (per sprint) integer assigned to a task, used by the team to refer to that task. " sqref="A17:A100" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="Exactly ONE team member may be responsible for any task, and they will receive grade credit for their work._x000a__x000a_If you have more than one person on your team, each member MUST select their initials for each task the agree to perform. Use this to ensure that " sqref="C17:C100" xr:uid="{00000000-0002-0000-0100-000002000000}">
-      <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
     <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong Value" error="This cell may only contain a valid status value (hint: use the drop-down selection list) or be left blank (hint: use the Delete key)" promptTitle="Implementation Status" prompt="Leave blank until task is begun._x000a_Select &quot;In Work&quot; when started (for long tasks only)._x000a_Select Completed ONLY when this task is done._x000a_    Select &quot;Completed Day 1&quot; if finished on the first day, and_x000a_    similarly for &quot;Completed on Day 2&quot; et. al." sqref="E17:E100" xr:uid="{00000000-0002-0000-0100-000003000000}">
@@ -8325,7 +8347,7 @@
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Select Feature ID from Product Backlog" prompt="The list contains the Feature IDs from the same column on the Product Backlog tab._x000a__x000a_For each (ahem) Feature ID, create one or more rows in this table representing the tasks you need to complete to implement that feature._x000a__x000a_For example, for a &quot;Provide Help " xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Product Backlog'!$A$24:$A$98</xm:f>
@@ -8334,6 +8356,12 @@
             <xm:f>0</xm:f>
           </x14:formula2>
           <xm:sqref>B17:B100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A046F40A-008F-AB47-BCA7-7B00CE7522EB}">
+          <x14:formula1>
+            <xm:f>'Product Backlog'!$H$5:$H$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>C17:C100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8346,7 +8374,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
@@ -8377,7 +8405,7 @@
     </row>
     <row r="2" spans="1:1024" s="33" customFormat="1">
       <c r="A2" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="34">
         <f>'Sprint 01 Backlog'!B3</f>
@@ -8385,7 +8413,7 @@
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -8394,7 +8422,7 @@
     </row>
     <row r="3" spans="1:1024" s="33" customFormat="1">
       <c r="A3" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="34">
         <f>B2+7</f>
@@ -8409,10 +8437,10 @@
     </row>
     <row r="4" spans="1:1024" s="33" customFormat="1">
       <c r="A4" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -8437,7 +8465,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
@@ -8447,7 +8475,7 @@
     </row>
     <row r="7" spans="1:1024" s="33" customFormat="1">
       <c r="A7" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="31">
         <f>COUNTA(D17:D995)</f>
@@ -8462,7 +8490,7 @@
     </row>
     <row r="8" spans="1:1024" s="33" customFormat="1">
       <c r="A8" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="31">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
@@ -8480,7 +8508,7 @@
     </row>
     <row r="9" spans="1:1024" s="33" customFormat="1">
       <c r="A9" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="31">
         <f t="shared" si="0"/>
@@ -8498,7 +8526,7 @@
     </row>
     <row r="10" spans="1:1024" s="33" customFormat="1">
       <c r="A10" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="31">
         <f t="shared" si="0"/>
@@ -8516,7 +8544,7 @@
     </row>
     <row r="11" spans="1:1024" s="33" customFormat="1">
       <c r="A11" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="31">
         <f t="shared" si="0"/>
@@ -8534,7 +8562,7 @@
     </row>
     <row r="12" spans="1:1024" s="33" customFormat="1">
       <c r="A12" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
@@ -8552,7 +8580,7 @@
     </row>
     <row r="13" spans="1:1024" s="33" customFormat="1">
       <c r="A13" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
@@ -8570,7 +8598,7 @@
     </row>
     <row r="14" spans="1:1024" s="33" customFormat="1">
       <c r="A14" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
@@ -8598,16 +8626,16 @@
     </row>
     <row r="16" spans="1:1024">
       <c r="A16" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="38" t="s">
         <v>144</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>145</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>25</v>
@@ -8622,7 +8650,7 @@
       </c>
       <c r="B17" s="39"/>
       <c r="D17" s="40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="41"/>
     </row>
@@ -9374,7 +9402,7 @@
     </row>
     <row r="2" spans="1:1024" s="33" customFormat="1">
       <c r="A2" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="34">
         <f>'Sprint 02 Backlog'!B2+7</f>
@@ -9382,7 +9410,7 @@
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -9391,7 +9419,7 @@
     </row>
     <row r="3" spans="1:1024" s="33" customFormat="1">
       <c r="A3" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="34">
         <f>B2+7</f>
@@ -9406,10 +9434,10 @@
     </row>
     <row r="4" spans="1:1024" s="33" customFormat="1">
       <c r="A4" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -9434,7 +9462,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
@@ -9444,7 +9472,7 @@
     </row>
     <row r="7" spans="1:1024" s="33" customFormat="1">
       <c r="A7" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="31">
         <f>COUNTA(D17:D995)</f>
@@ -9459,7 +9487,7 @@
     </row>
     <row r="8" spans="1:1024" s="33" customFormat="1">
       <c r="A8" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="31">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
@@ -9477,7 +9505,7 @@
     </row>
     <row r="9" spans="1:1024" s="33" customFormat="1">
       <c r="A9" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="31">
         <f t="shared" si="0"/>
@@ -9495,7 +9523,7 @@
     </row>
     <row r="10" spans="1:1024" s="33" customFormat="1">
       <c r="A10" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="31">
         <f t="shared" si="0"/>
@@ -9513,7 +9541,7 @@
     </row>
     <row r="11" spans="1:1024" s="33" customFormat="1">
       <c r="A11" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="31">
         <f t="shared" si="0"/>
@@ -9531,7 +9559,7 @@
     </row>
     <row r="12" spans="1:1024" s="33" customFormat="1">
       <c r="A12" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
@@ -9549,7 +9577,7 @@
     </row>
     <row r="13" spans="1:1024" s="33" customFormat="1">
       <c r="A13" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
@@ -9567,7 +9595,7 @@
     </row>
     <row r="14" spans="1:1024" s="33" customFormat="1">
       <c r="A14" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
@@ -9595,16 +9623,16 @@
     </row>
     <row r="16" spans="1:1024">
       <c r="A16" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="38" t="s">
         <v>144</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>145</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>25</v>
@@ -9619,7 +9647,7 @@
       </c>
       <c r="B17" s="39"/>
       <c r="D17" s="40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="41"/>
     </row>
@@ -10371,14 +10399,14 @@
     </row>
     <row r="2" spans="1:1024" s="33" customFormat="1">
       <c r="A2" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="34">
         <v>44663</v>
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -10387,7 +10415,7 @@
     </row>
     <row r="3" spans="1:1024" s="33" customFormat="1">
       <c r="A3" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="34">
         <f>B2+7</f>
@@ -10402,10 +10430,10 @@
     </row>
     <row r="4" spans="1:1024" s="33" customFormat="1">
       <c r="A4" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -10430,7 +10458,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
@@ -10440,7 +10468,7 @@
     </row>
     <row r="7" spans="1:1024" s="33" customFormat="1">
       <c r="A7" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="31">
         <f>COUNTA(D17:D995)</f>
@@ -10455,7 +10483,7 @@
     </row>
     <row r="8" spans="1:1024" s="33" customFormat="1">
       <c r="A8" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="31">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
@@ -10473,7 +10501,7 @@
     </row>
     <row r="9" spans="1:1024" s="33" customFormat="1">
       <c r="A9" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="31">
         <f t="shared" si="0"/>
@@ -10491,7 +10519,7 @@
     </row>
     <row r="10" spans="1:1024" s="33" customFormat="1">
       <c r="A10" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="31">
         <f t="shared" si="0"/>
@@ -10509,7 +10537,7 @@
     </row>
     <row r="11" spans="1:1024" s="33" customFormat="1">
       <c r="A11" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="31">
         <f t="shared" si="0"/>
@@ -10527,7 +10555,7 @@
     </row>
     <row r="12" spans="1:1024" s="33" customFormat="1">
       <c r="A12" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
@@ -10545,7 +10573,7 @@
     </row>
     <row r="13" spans="1:1024" s="33" customFormat="1">
       <c r="A13" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
@@ -10563,7 +10591,7 @@
     </row>
     <row r="14" spans="1:1024" s="33" customFormat="1">
       <c r="A14" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
@@ -10591,16 +10619,16 @@
     </row>
     <row r="16" spans="1:1024">
       <c r="A16" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="38" t="s">
         <v>144</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>145</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>25</v>
@@ -10615,7 +10643,7 @@
       </c>
       <c r="B17" s="39"/>
       <c r="D17" s="40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="41"/>
     </row>
@@ -11367,7 +11395,7 @@
     </row>
     <row r="2" spans="1:1024" s="33" customFormat="1">
       <c r="A2" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="34">
         <f>'Sprint 04 Backlog'!B2+7</f>
@@ -11375,7 +11403,7 @@
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="31"/>
       <c r="F2" s="31"/>
@@ -11384,7 +11412,7 @@
     </row>
     <row r="3" spans="1:1024" s="33" customFormat="1">
       <c r="A3" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B3" s="34">
         <f>B2+7</f>
@@ -11399,10 +11427,10 @@
     </row>
     <row r="4" spans="1:1024" s="33" customFormat="1">
       <c r="A4" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="31"/>
       <c r="D4" s="31"/>
@@ -11427,7 +11455,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
@@ -11437,7 +11465,7 @@
     </row>
     <row r="7" spans="1:1024" s="33" customFormat="1">
       <c r="A7" s="31" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="31">
         <f>COUNTA(D17:D995)</f>
@@ -11452,7 +11480,7 @@
     </row>
     <row r="8" spans="1:1024" s="33" customFormat="1">
       <c r="A8" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B8" s="31">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
@@ -11470,7 +11498,7 @@
     </row>
     <row r="9" spans="1:1024" s="33" customFormat="1">
       <c r="A9" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B9" s="31">
         <f t="shared" si="0"/>
@@ -11488,7 +11516,7 @@
     </row>
     <row r="10" spans="1:1024" s="33" customFormat="1">
       <c r="A10" s="31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B10" s="31">
         <f t="shared" si="0"/>
@@ -11506,7 +11534,7 @@
     </row>
     <row r="11" spans="1:1024" s="33" customFormat="1">
       <c r="A11" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="31">
         <f t="shared" si="0"/>
@@ -11524,7 +11552,7 @@
     </row>
     <row r="12" spans="1:1024" s="33" customFormat="1">
       <c r="A12" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
@@ -11542,7 +11570,7 @@
     </row>
     <row r="13" spans="1:1024" s="33" customFormat="1">
       <c r="A13" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
@@ -11560,7 +11588,7 @@
     </row>
     <row r="14" spans="1:1024" s="33" customFormat="1">
       <c r="A14" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
@@ -11588,16 +11616,16 @@
     </row>
     <row r="16" spans="1:1024">
       <c r="A16" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="38" t="s">
         <v>144</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>145</v>
       </c>
       <c r="E16" s="38" t="s">
         <v>25</v>
@@ -11612,7 +11640,7 @@
       </c>
       <c r="B17" s="39"/>
       <c r="D17" s="40" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E17" s="41"/>
     </row>

</xml_diff>